<commit_message>
add s2 analysis file
</commit_message>
<xml_diff>
--- a/crkaide_working_docs/MRIP_Survey_Variables.xlsx
+++ b/crkaide_working_docs/MRIP_Survey_Variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cjreinhardt/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://illinoisstateuniversity-my.sharepoint.com/personal/crkaide_ilstu_edu/Documents/Vanderbilt/Vanderbilt/Assignments/20_Final_Project/Team-Frist-Center/crkaide_working_docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E1939B0D-19E3-2E41-BD0B-060BD4CA29C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="8_{E1939B0D-19E3-2E41-BD0B-060BD4CA29C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{684EDE89-D18E-2C43-A7AD-AE38A6090908}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2"/>
+    <workbookView xWindow="27020" yWindow="460" windowWidth="23040" windowHeight="26840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="size_begin2013w2" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="trip_pre2013w2" sheetId="7" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">trip_begin2013w2!$A$1:$A$79</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">trip_begin2013w2!$A$1:$G$79</definedName>
     <definedName name="catch">catch_begin2013w2!$A$1:$F$29</definedName>
     <definedName name="catch_pre2013w2">catch_pre2013w2!$A$1:$F$27</definedName>
     <definedName name="size">size_begin2013w2!$A$1:$F$22</definedName>
@@ -30,15 +30,6 @@
     <definedName name="trip_pre2013w2">trip_pre2013w2!$A$1:$F$77</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -1273,7 +1264,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
@@ -1303,7 +1294,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1316,8 +1307,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1343,13 +1346,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1380,32 +1398,59 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCC0DA"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -1819,7 +1864,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
@@ -2327,7 +2372,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
@@ -2968,589 +3013,612 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:H79"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:IV25"/>
+      <selection activeCell="A32" sqref="A32:XFD32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="16.5" customWidth="1"/>
-    <col min="3" max="3" width="6.1640625" customWidth="1"/>
-    <col min="4" max="4" width="8.83203125" customWidth="1"/>
-    <col min="5" max="5" width="48.33203125" customWidth="1"/>
-    <col min="6" max="6" width="9.1640625" customWidth="1"/>
-    <col min="7" max="7" width="90" customWidth="1"/>
-    <col min="8" max="8" width="4.6640625" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="11" style="17" customWidth="1"/>
+    <col min="2" max="2" width="16.5" style="17" customWidth="1"/>
+    <col min="3" max="3" width="6.1640625" style="17" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" style="17" customWidth="1"/>
+    <col min="5" max="5" width="48.33203125" style="17" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" style="17" customWidth="1"/>
+    <col min="7" max="7" width="66.83203125" style="16" customWidth="1"/>
+    <col min="8" max="8" width="25" customWidth="1"/>
+    <col min="9" max="16384" width="9.1640625" style="17"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="19" t="s">
         <v>248</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="19" t="s">
         <v>170</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="19" t="s">
         <v>235</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="19" t="s">
         <v>286</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="20" t="s">
         <v>176</v>
       </c>
       <c r="H1" s="8"/>
     </row>
-    <row r="2" spans="1:8" s="16" customFormat="1" ht="28" x14ac:dyDescent="0.15">
-      <c r="A2" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="B2" s="13" t="s">
+    <row r="2" spans="1:8" s="18" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A2" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="C2" s="13">
-        <v>1</v>
-      </c>
-      <c r="D2" s="13">
-        <v>8</v>
-      </c>
-      <c r="E2" s="13" t="s">
+      <c r="C2" s="21">
+        <v>1</v>
+      </c>
+      <c r="D2" s="21">
+        <v>8</v>
+      </c>
+      <c r="E2" s="21" t="s">
         <v>267</v>
       </c>
-      <c r="F2" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="G2" s="14" t="s">
+      <c r="F2" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="G2" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="H2" s="15"/>
-    </row>
-    <row r="3" spans="1:8" ht="84" x14ac:dyDescent="0.15">
-      <c r="A3" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="B3" s="12" t="s">
+      <c r="H2" s="9"/>
+    </row>
+    <row r="3" spans="1:8" s="18" customFormat="1" ht="84" x14ac:dyDescent="0.15">
+      <c r="A3" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="C3" s="12">
-        <v>2</v>
-      </c>
-      <c r="D3" s="12">
-        <v>1</v>
-      </c>
-      <c r="E3" s="12" t="s">
+      <c r="C3" s="21">
+        <v>2</v>
+      </c>
+      <c r="D3" s="21">
+        <v>1</v>
+      </c>
+      <c r="E3" s="21" t="s">
         <v>294</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="G3" s="17" t="s">
+      <c r="G3" s="22" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="56" x14ac:dyDescent="0.15">
-      <c r="A4" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="B4" s="12" t="s">
+      <c r="H3" s="15"/>
+    </row>
+    <row r="4" spans="1:8" s="18" customFormat="1" ht="56" x14ac:dyDescent="0.15">
+      <c r="A4" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="21" t="s">
         <v>203</v>
       </c>
-      <c r="C4" s="12">
-        <v>1</v>
-      </c>
-      <c r="D4" s="12">
-        <v>8</v>
-      </c>
-      <c r="E4" s="12" t="s">
+      <c r="C4" s="21">
+        <v>1</v>
+      </c>
+      <c r="D4" s="21">
+        <v>8</v>
+      </c>
+      <c r="E4" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="F4" s="16"/>
-      <c r="G4" s="17" t="s">
+      <c r="F4" s="23"/>
+      <c r="G4" s="25" t="s">
         <v>197</v>
       </c>
       <c r="H4" s="7"/>
     </row>
-    <row r="5" spans="1:8" ht="28" x14ac:dyDescent="0.15">
-      <c r="A5" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="B5" s="12" t="s">
+    <row r="5" spans="1:8" s="18" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A5" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="21" t="s">
         <v>204</v>
       </c>
-      <c r="C5" s="12">
-        <v>1</v>
-      </c>
-      <c r="D5" s="12">
-        <v>8</v>
-      </c>
-      <c r="E5" s="12" t="s">
+      <c r="C5" s="21">
+        <v>1</v>
+      </c>
+      <c r="D5" s="21">
+        <v>8</v>
+      </c>
+      <c r="E5" s="21" t="s">
         <v>298</v>
       </c>
-      <c r="F5" s="16"/>
-      <c r="G5" s="17" t="s">
+      <c r="F5" s="23"/>
+      <c r="G5" s="22" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="56" x14ac:dyDescent="0.15">
-      <c r="A6" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="B6" s="12" t="s">
+      <c r="H5" s="15"/>
+    </row>
+    <row r="6" spans="1:8" s="18" customFormat="1" ht="56" x14ac:dyDescent="0.15">
+      <c r="A6" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" s="21" t="s">
         <v>215</v>
       </c>
-      <c r="C6" s="12">
-        <v>1</v>
-      </c>
-      <c r="D6" s="12">
-        <v>8</v>
-      </c>
-      <c r="E6" s="12" t="s">
+      <c r="C6" s="21">
+        <v>1</v>
+      </c>
+      <c r="D6" s="21">
+        <v>8</v>
+      </c>
+      <c r="E6" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="F6" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="G6" s="17" t="s">
+      <c r="F6" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="G6" s="22" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" s="16" customFormat="1" ht="84" x14ac:dyDescent="0.15">
-      <c r="A7" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="B7" s="12" t="s">
+      <c r="H6" s="15"/>
+    </row>
+    <row r="7" spans="1:8" s="18" customFormat="1" ht="84" x14ac:dyDescent="0.15">
+      <c r="A7" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="21" t="s">
         <v>265</v>
       </c>
-      <c r="C7" s="12">
-        <v>2</v>
-      </c>
-      <c r="D7" s="12">
-        <v>1</v>
-      </c>
-      <c r="E7" s="12" t="s">
+      <c r="C7" s="21">
+        <v>2</v>
+      </c>
+      <c r="D7" s="21">
+        <v>1</v>
+      </c>
+      <c r="E7" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="F7" s="23"/>
+      <c r="G7" s="22" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" s="16" customFormat="1" ht="84" x14ac:dyDescent="0.15">
-      <c r="A8" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="B8" s="12" t="s">
+      <c r="H7" s="15"/>
+    </row>
+    <row r="8" spans="1:8" s="18" customFormat="1" ht="84" x14ac:dyDescent="0.15">
+      <c r="A8" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="21" t="s">
         <v>232</v>
       </c>
-      <c r="C8" s="12">
-        <v>2</v>
-      </c>
-      <c r="D8" s="12">
-        <v>1</v>
-      </c>
-      <c r="E8" s="12" t="s">
+      <c r="C8" s="21">
+        <v>2</v>
+      </c>
+      <c r="D8" s="21">
+        <v>1</v>
+      </c>
+      <c r="E8" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="G8" s="22" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="14" x14ac:dyDescent="0.15">
-      <c r="A9" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="B9" s="12" t="s">
+      <c r="H8" s="15"/>
+    </row>
+    <row r="9" spans="1:8" s="18" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A9" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="12">
-        <v>1</v>
-      </c>
-      <c r="D9" s="12">
-        <v>8</v>
-      </c>
-      <c r="E9" s="12" t="s">
+      <c r="C9" s="21">
+        <v>1</v>
+      </c>
+      <c r="D9" s="21">
+        <v>8</v>
+      </c>
+      <c r="E9" s="21" t="s">
         <v>243</v>
       </c>
-      <c r="F9" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="G9" s="17" t="s">
+      <c r="F9" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="G9" s="22" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" s="16" customFormat="1" ht="182" x14ac:dyDescent="0.15">
-      <c r="A10" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="B10" s="12" t="s">
+      <c r="H9" s="15"/>
+    </row>
+    <row r="10" spans="1:8" s="18" customFormat="1" ht="182" x14ac:dyDescent="0.15">
+      <c r="A10" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="12">
-        <v>1</v>
-      </c>
-      <c r="D10" s="12">
-        <v>8</v>
-      </c>
-      <c r="E10" s="12" t="s">
+      <c r="C10" s="21">
+        <v>1</v>
+      </c>
+      <c r="D10" s="21">
+        <v>8</v>
+      </c>
+      <c r="E10" s="21" t="s">
         <v>289</v>
       </c>
-      <c r="F10" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="G10" s="17" t="s">
+      <c r="F10" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="G10" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="H10" s="18"/>
-    </row>
-    <row r="11" spans="1:8" s="16" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="A11" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="B11" s="12" t="s">
+      <c r="H10" s="7"/>
+    </row>
+    <row r="11" spans="1:8" s="18" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A11" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" s="21" t="s">
         <v>288</v>
       </c>
-      <c r="C11" s="12">
-        <v>1</v>
-      </c>
-      <c r="D11" s="12">
-        <v>8</v>
-      </c>
-      <c r="E11" s="12" t="s">
+      <c r="C11" s="21">
+        <v>1</v>
+      </c>
+      <c r="D11" s="21">
+        <v>8</v>
+      </c>
+      <c r="E11" s="21" t="s">
         <v>249</v>
       </c>
-      <c r="G11" s="17" t="s">
+      <c r="F11" s="23"/>
+      <c r="G11" s="22" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="42" x14ac:dyDescent="0.15">
-      <c r="A12" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="B12" s="12" t="s">
+      <c r="H11" s="15"/>
+    </row>
+    <row r="12" spans="1:8" s="18" customFormat="1" ht="42" x14ac:dyDescent="0.15">
+      <c r="A12" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="C12" s="12">
-        <v>1</v>
-      </c>
-      <c r="D12" s="12">
-        <v>8</v>
-      </c>
-      <c r="E12" s="12" t="s">
+      <c r="C12" s="21">
+        <v>1</v>
+      </c>
+      <c r="D12" s="21">
+        <v>8</v>
+      </c>
+      <c r="E12" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="F12" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="G12" s="17" t="s">
+      <c r="F12" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="G12" s="22" t="s">
         <v>281</v>
       </c>
       <c r="H12" s="7"/>
     </row>
-    <row r="13" spans="1:8" ht="70" x14ac:dyDescent="0.15">
-      <c r="A13" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="B13" s="12" t="s">
+    <row r="13" spans="1:8" s="18" customFormat="1" ht="84" x14ac:dyDescent="0.15">
+      <c r="A13" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" s="21" t="s">
         <v>155</v>
       </c>
-      <c r="C13" s="12">
-        <v>2</v>
-      </c>
-      <c r="D13" s="12">
-        <v>2</v>
-      </c>
-      <c r="E13" s="12" t="s">
+      <c r="C13" s="21">
+        <v>2</v>
+      </c>
+      <c r="D13" s="21">
+        <v>2</v>
+      </c>
+      <c r="E13" s="21" t="s">
         <v>255</v>
       </c>
-      <c r="F13" s="16"/>
-      <c r="G13" s="17" t="s">
+      <c r="F13" s="23"/>
+      <c r="G13" s="22" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="126" x14ac:dyDescent="0.15">
-      <c r="A14" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="B14" s="12" t="s">
+      <c r="H13" s="15"/>
+    </row>
+    <row r="14" spans="1:8" s="18" customFormat="1" ht="126" x14ac:dyDescent="0.15">
+      <c r="A14" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="12">
-        <v>2</v>
-      </c>
-      <c r="D14" s="12">
-        <v>1</v>
-      </c>
-      <c r="E14" s="12" t="s">
+      <c r="C14" s="21">
+        <v>2</v>
+      </c>
+      <c r="D14" s="21">
+        <v>1</v>
+      </c>
+      <c r="E14" s="21" t="s">
         <v>141</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="G14" s="17" t="s">
+      <c r="G14" s="22" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" ht="98" x14ac:dyDescent="0.15">
-      <c r="A15" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="B15" s="12" t="s">
+      <c r="H14" s="15"/>
+    </row>
+    <row r="15" spans="1:8" s="18" customFormat="1" ht="98" x14ac:dyDescent="0.15">
+      <c r="A15" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="C15" s="12">
-        <v>2</v>
-      </c>
-      <c r="D15" s="12">
-        <v>1</v>
-      </c>
-      <c r="E15" s="12" t="s">
+      <c r="C15" s="21">
+        <v>2</v>
+      </c>
+      <c r="D15" s="21">
+        <v>1</v>
+      </c>
+      <c r="E15" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="F15" s="12" t="s">
+      <c r="F15" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="G15" s="17" t="s">
+      <c r="G15" s="22" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" ht="154" x14ac:dyDescent="0.15">
-      <c r="A16" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="B16" s="12" t="s">
+      <c r="H15" s="15"/>
+    </row>
+    <row r="16" spans="1:8" s="18" customFormat="1" ht="154" x14ac:dyDescent="0.15">
+      <c r="A16" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="C16" s="12">
-        <v>2</v>
-      </c>
-      <c r="D16" s="12">
+      <c r="C16" s="21">
+        <v>2</v>
+      </c>
+      <c r="D16" s="21">
         <v>5</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E16" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="F16" s="18"/>
-      <c r="G16" s="17" t="s">
+      <c r="F16" s="24"/>
+      <c r="G16" s="22" t="s">
         <v>193</v>
       </c>
       <c r="H16" s="7"/>
     </row>
-    <row r="17" spans="1:8" ht="56" x14ac:dyDescent="0.15">
-      <c r="A17" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="B17" s="12" t="s">
+    <row r="17" spans="1:8" s="18" customFormat="1" ht="70" x14ac:dyDescent="0.15">
+      <c r="A17" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="12">
-        <v>2</v>
-      </c>
-      <c r="D17" s="12">
-        <v>2</v>
-      </c>
-      <c r="E17" s="18" t="s">
+      <c r="C17" s="21">
+        <v>2</v>
+      </c>
+      <c r="D17" s="21">
+        <v>2</v>
+      </c>
+      <c r="E17" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="F17" s="16"/>
-      <c r="G17" s="17" t="s">
+      <c r="F17" s="23"/>
+      <c r="G17" s="22" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="14" x14ac:dyDescent="0.15">
-      <c r="A18" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="12">
-        <v>2</v>
-      </c>
-      <c r="D18" s="12">
+      <c r="H17" s="15"/>
+    </row>
+    <row r="18" spans="1:8" s="18" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A18" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="21">
+        <v>2</v>
+      </c>
+      <c r="D18" s="21">
         <v>10</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="E18" s="21" t="s">
         <v>218</v>
       </c>
-      <c r="F18" s="12" t="s">
+      <c r="F18" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="G18" s="17" t="s">
+      <c r="G18" s="22" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="14" x14ac:dyDescent="0.15">
-      <c r="A19" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="B19" s="12" t="s">
+      <c r="H18" s="15"/>
+    </row>
+    <row r="19" spans="1:8" s="18" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A19" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="12">
-        <v>2</v>
-      </c>
-      <c r="D19" s="12">
+      <c r="C19" s="21">
+        <v>2</v>
+      </c>
+      <c r="D19" s="21">
         <v>10</v>
       </c>
-      <c r="E19" s="12" t="s">
+      <c r="E19" s="21" t="s">
         <v>162</v>
       </c>
-      <c r="F19" s="12" t="s">
+      <c r="F19" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="G19" s="17" t="s">
+      <c r="G19" s="22" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" s="16" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="A20" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="B20" s="12" t="s">
+      <c r="H19" s="15"/>
+    </row>
+    <row r="20" spans="1:8" s="18" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A20" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" s="21" t="s">
         <v>306</v>
       </c>
-      <c r="C20" s="12">
-        <v>1</v>
-      </c>
-      <c r="D20" s="12">
-        <v>8</v>
-      </c>
-      <c r="E20" s="12" t="s">
+      <c r="C20" s="21">
+        <v>1</v>
+      </c>
+      <c r="D20" s="21">
+        <v>8</v>
+      </c>
+      <c r="E20" s="21" t="s">
         <v>306</v>
       </c>
-      <c r="F20" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="G20" s="17" t="s">
+      <c r="F20" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="G20" s="22" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" s="16" customFormat="1" ht="70" x14ac:dyDescent="0.15">
-      <c r="A21" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="B21" s="12" t="s">
+      <c r="H20" s="15"/>
+    </row>
+    <row r="21" spans="1:8" s="18" customFormat="1" ht="70" x14ac:dyDescent="0.15">
+      <c r="A21" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" s="21" t="s">
         <v>202</v>
       </c>
-      <c r="C21" s="12">
-        <v>1</v>
-      </c>
-      <c r="D21" s="12">
-        <v>8</v>
-      </c>
-      <c r="E21" s="12" t="s">
+      <c r="C21" s="21">
+        <v>1</v>
+      </c>
+      <c r="D21" s="21">
+        <v>8</v>
+      </c>
+      <c r="E21" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="F21" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="G21" s="17" t="s">
+      <c r="F21" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="G21" s="22" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" ht="98" x14ac:dyDescent="0.15">
-      <c r="A22" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="B22" s="12" t="s">
+      <c r="H21" s="15"/>
+    </row>
+    <row r="22" spans="1:8" s="18" customFormat="1" ht="98" x14ac:dyDescent="0.15">
+      <c r="A22" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" s="21" t="s">
         <v>252</v>
       </c>
-      <c r="C22" s="12">
-        <v>1</v>
-      </c>
-      <c r="D22" s="12">
-        <v>8</v>
-      </c>
-      <c r="E22" s="12" t="s">
+      <c r="C22" s="21">
+        <v>1</v>
+      </c>
+      <c r="D22" s="21">
+        <v>8</v>
+      </c>
+      <c r="E22" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="F22" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="G22" s="17" t="s">
+      <c r="F22" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="G22" s="22" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" ht="28" x14ac:dyDescent="0.15">
-      <c r="A23" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="B23" s="12" t="s">
+      <c r="H22" s="15"/>
+    </row>
+    <row r="23" spans="1:8" s="18" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A23" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="C23" s="12">
-        <v>1</v>
-      </c>
-      <c r="D23" s="12">
-        <v>8</v>
-      </c>
-      <c r="E23" s="12" t="s">
+      <c r="C23" s="21">
+        <v>1</v>
+      </c>
+      <c r="D23" s="21">
+        <v>8</v>
+      </c>
+      <c r="E23" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="F23" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="G23" s="17" t="s">
+      <c r="F23" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="G23" s="22" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" ht="14" x14ac:dyDescent="0.15">
-      <c r="A24" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="B24" s="12" t="s">
+      <c r="H23" s="15"/>
+    </row>
+    <row r="24" spans="1:8" s="18" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A24" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" s="21" t="s">
         <v>266</v>
       </c>
-      <c r="C24" s="12">
-        <v>2</v>
-      </c>
-      <c r="D24" s="12">
+      <c r="C24" s="21">
+        <v>2</v>
+      </c>
+      <c r="D24" s="21">
         <v>7</v>
       </c>
-      <c r="E24" s="12" t="s">
+      <c r="E24" s="21" t="s">
         <v>218</v>
       </c>
-      <c r="F24" s="12" t="s">
+      <c r="F24" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="G24" s="17" t="s">
+      <c r="G24" s="22" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" ht="98" x14ac:dyDescent="0.15">
-      <c r="A25" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="B25" s="12" t="s">
+      <c r="H24" s="15"/>
+    </row>
+    <row r="25" spans="1:8" s="18" customFormat="1" ht="98" x14ac:dyDescent="0.15">
+      <c r="A25" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" s="21" t="s">
         <v>283</v>
       </c>
-      <c r="C25" s="12">
-        <v>1</v>
-      </c>
-      <c r="D25" s="12">
-        <v>8</v>
-      </c>
-      <c r="E25" s="12" t="s">
+      <c r="C25" s="21">
+        <v>1</v>
+      </c>
+      <c r="D25" s="21">
+        <v>8</v>
+      </c>
+      <c r="E25" s="21" t="s">
         <v>282</v>
       </c>
-      <c r="F25" s="16"/>
-      <c r="G25" s="17" t="s">
+      <c r="F25" s="23"/>
+      <c r="G25" s="22" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" s="16" customFormat="1" ht="42" x14ac:dyDescent="0.15">
+      <c r="H25" s="15"/>
+    </row>
+    <row r="26" spans="1:8" s="12" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.15">
       <c r="A26" s="5" t="s">
         <v>68</v>
       </c>
@@ -3573,52 +3641,53 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="16" customFormat="1" ht="28" x14ac:dyDescent="0.15">
-      <c r="A27" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B27" s="5" t="s">
+    <row r="27" spans="1:8" s="18" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A27" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" s="21" t="s">
         <v>130</v>
       </c>
-      <c r="C27" s="5">
-        <v>1</v>
-      </c>
-      <c r="D27" s="5">
-        <v>8</v>
-      </c>
-      <c r="E27" s="5" t="s">
+      <c r="C27" s="21">
+        <v>1</v>
+      </c>
+      <c r="D27" s="21">
+        <v>8</v>
+      </c>
+      <c r="E27" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="F27"/>
-      <c r="G27" s="6" t="s">
+      <c r="F27" s="23"/>
+      <c r="G27" s="22" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" ht="371" x14ac:dyDescent="0.15">
-      <c r="A28" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B28" s="5" t="s">
+      <c r="H27" s="15"/>
+    </row>
+    <row r="28" spans="1:8" s="18" customFormat="1" ht="371" x14ac:dyDescent="0.15">
+      <c r="A28" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="C28" s="5">
-        <v>2</v>
-      </c>
-      <c r="D28" s="5">
-        <v>1</v>
-      </c>
-      <c r="E28" s="5" t="s">
+      <c r="C28" s="21">
+        <v>2</v>
+      </c>
+      <c r="D28" s="21">
+        <v>1</v>
+      </c>
+      <c r="E28" s="21" t="s">
         <v>272</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="F28" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="G28" s="6" t="s">
+      <c r="G28" s="22" t="s">
         <v>134</v>
       </c>
       <c r="H28" s="7"/>
     </row>
-    <row r="29" spans="1:8" s="16" customFormat="1" ht="397" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:8" s="12" customFormat="1" ht="397" hidden="1" x14ac:dyDescent="0.15">
       <c r="A29" s="5" t="s">
         <v>68</v>
       </c>
@@ -3638,9 +3707,9 @@
       <c r="G29" s="6" t="s">
         <v>296</v>
       </c>
-      <c r="H29" s="18"/>
-    </row>
-    <row r="30" spans="1:8" s="16" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="H29" s="13"/>
+    </row>
+    <row r="30" spans="1:8" s="12" customFormat="1" ht="14" hidden="1" x14ac:dyDescent="0.15">
       <c r="A30" s="5" t="s">
         <v>68</v>
       </c>
@@ -3661,7 +3730,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="84" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:8" customFormat="1" ht="84" hidden="1" x14ac:dyDescent="0.15">
       <c r="A31" s="5" t="s">
         <v>68</v>
       </c>
@@ -3682,55 +3751,55 @@
       </c>
       <c r="H31" s="7"/>
     </row>
-    <row r="32" spans="1:8" ht="28" x14ac:dyDescent="0.15">
-      <c r="A32" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B32" s="5" t="s">
+    <row r="32" spans="1:8" s="18" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A32" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B32" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="C32" s="5">
-        <v>1</v>
-      </c>
-      <c r="D32" s="5">
-        <v>8</v>
-      </c>
-      <c r="E32" s="5" t="s">
+      <c r="C32" s="21">
+        <v>1</v>
+      </c>
+      <c r="D32" s="21">
+        <v>8</v>
+      </c>
+      <c r="E32" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="F32" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="G32" s="6" t="s">
+      <c r="F32" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="G32" s="22" t="s">
         <v>109</v>
       </c>
       <c r="H32" s="7"/>
     </row>
-    <row r="33" spans="1:8" s="16" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="A33" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B33" s="5" t="s">
+    <row r="33" spans="1:8" s="18" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A33" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B33" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="C33" s="5">
-        <v>1</v>
-      </c>
-      <c r="D33" s="5">
-        <v>8</v>
-      </c>
-      <c r="E33" s="5" t="s">
+      <c r="C33" s="21">
+        <v>1</v>
+      </c>
+      <c r="D33" s="21">
+        <v>8</v>
+      </c>
+      <c r="E33" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="F33" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="G33" s="6" t="s">
+      <c r="F33" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="G33" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="H33" s="18"/>
-    </row>
-    <row r="34" spans="1:8" ht="14" x14ac:dyDescent="0.15">
+      <c r="H33" s="7"/>
+    </row>
+    <row r="34" spans="1:8" customFormat="1" ht="14" hidden="1" x14ac:dyDescent="0.15">
       <c r="A34" s="5" t="s">
         <v>68</v>
       </c>
@@ -3754,7 +3823,7 @@
       </c>
       <c r="H34" s="7"/>
     </row>
-    <row r="35" spans="1:8" ht="70" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:8" customFormat="1" ht="70" hidden="1" x14ac:dyDescent="0.15">
       <c r="A35" s="5" t="s">
         <v>68</v>
       </c>
@@ -3774,7 +3843,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="42" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:8" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.15">
       <c r="A36" s="5" t="s">
         <v>68</v>
       </c>
@@ -3794,7 +3863,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="37" spans="1:8" s="16" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:8" s="12" customFormat="1" ht="14" hidden="1" x14ac:dyDescent="0.15">
       <c r="A37" s="5" t="s">
         <v>68</v>
       </c>
@@ -3815,7 +3884,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="38" spans="1:8" s="16" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:8" s="12" customFormat="1" ht="14" hidden="1" x14ac:dyDescent="0.15">
       <c r="A38" s="5" t="s">
         <v>68</v>
       </c>
@@ -3836,7 +3905,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="39" spans="1:8" s="16" customFormat="1" ht="56" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:8" s="12" customFormat="1" ht="56" hidden="1" x14ac:dyDescent="0.15">
       <c r="A39" s="5" t="s">
         <v>68</v>
       </c>
@@ -3859,7 +3928,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="42" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:8" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.15">
       <c r="A40" s="5" t="s">
         <v>68</v>
       </c>
@@ -3882,7 +3951,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="41" spans="1:8" s="16" customFormat="1" ht="42" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:8" s="12" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.15">
       <c r="A41" s="5" t="s">
         <v>68</v>
       </c>
@@ -3904,9 +3973,9 @@
       <c r="G41" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="H41" s="18"/>
-    </row>
-    <row r="42" spans="1:8" ht="56" x14ac:dyDescent="0.15">
+      <c r="H41" s="13"/>
+    </row>
+    <row r="42" spans="1:8" customFormat="1" ht="56" hidden="1" x14ac:dyDescent="0.15">
       <c r="A42" s="5" t="s">
         <v>68</v>
       </c>
@@ -3929,27 +3998,29 @@
         <v>259</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="56" x14ac:dyDescent="0.15">
-      <c r="A43" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B43" s="5" t="s">
+    <row r="43" spans="1:8" s="18" customFormat="1" ht="56" x14ac:dyDescent="0.15">
+      <c r="A43" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B43" s="21" t="s">
         <v>295</v>
       </c>
-      <c r="C43" s="5">
-        <v>1</v>
-      </c>
-      <c r="D43" s="5">
-        <v>8</v>
-      </c>
-      <c r="E43" s="5" t="s">
+      <c r="C43" s="21">
+        <v>1</v>
+      </c>
+      <c r="D43" s="21">
+        <v>8</v>
+      </c>
+      <c r="E43" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="G43" s="6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="84" x14ac:dyDescent="0.15">
+      <c r="F43" s="23"/>
+      <c r="G43" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="H43" s="15"/>
+    </row>
+    <row r="44" spans="1:8" customFormat="1" ht="84" hidden="1" x14ac:dyDescent="0.15">
       <c r="A44" s="5" t="s">
         <v>68</v>
       </c>
@@ -3972,7 +4043,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="14" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:8" customFormat="1" ht="14" hidden="1" x14ac:dyDescent="0.15">
       <c r="A45" s="5" t="s">
         <v>68</v>
       </c>
@@ -3995,7 +4066,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="14" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:8" customFormat="1" ht="14" hidden="1" x14ac:dyDescent="0.15">
       <c r="A46" s="5" t="s">
         <v>68</v>
       </c>
@@ -4016,7 +4087,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="56" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:8" customFormat="1" ht="56" hidden="1" x14ac:dyDescent="0.15">
       <c r="A47" s="5" t="s">
         <v>68</v>
       </c>
@@ -4039,7 +4110,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="182" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:8" customFormat="1" ht="182" hidden="1" x14ac:dyDescent="0.15">
       <c r="A48" s="5" t="s">
         <v>68</v>
       </c>
@@ -4062,7 +4133,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="70" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:8" customFormat="1" ht="70" hidden="1" x14ac:dyDescent="0.15">
       <c r="A49" s="5" t="s">
         <v>68</v>
       </c>
@@ -4082,7 +4153,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="14" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:8" customFormat="1" ht="14" hidden="1" x14ac:dyDescent="0.15">
       <c r="A50" s="5" t="s">
         <v>68</v>
       </c>
@@ -4102,7 +4173,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="14" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:8" customFormat="1" ht="14" hidden="1" x14ac:dyDescent="0.15">
       <c r="A51" s="5" t="s">
         <v>68</v>
       </c>
@@ -4123,7 +4194,7 @@
       </c>
       <c r="H51" s="7"/>
     </row>
-    <row r="52" spans="1:8" ht="42" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:8" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.15">
       <c r="A52" s="5" t="s">
         <v>68</v>
       </c>
@@ -4144,7 +4215,7 @@
       </c>
       <c r="H52" s="7"/>
     </row>
-    <row r="53" spans="1:8" ht="14" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:8" customFormat="1" ht="14" hidden="1" x14ac:dyDescent="0.15">
       <c r="A53" s="5" t="s">
         <v>68</v>
       </c>
@@ -4164,7 +4235,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="54" spans="1:8" s="16" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:8" s="12" customFormat="1" ht="14" hidden="1" x14ac:dyDescent="0.15">
       <c r="A54" s="5" t="s">
         <v>68</v>
       </c>
@@ -4187,7 +4258,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="55" spans="1:8" s="16" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:8" s="12" customFormat="1" ht="14" hidden="1" x14ac:dyDescent="0.15">
       <c r="A55" s="5" t="s">
         <v>68</v>
       </c>
@@ -4210,7 +4281,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="42" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:8" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.15">
       <c r="A56" s="5" t="s">
         <v>68</v>
       </c>
@@ -4233,7 +4304,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="42" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:8" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.15">
       <c r="A57" s="5" t="s">
         <v>68</v>
       </c>
@@ -4256,7 +4327,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="14" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:8" customFormat="1" ht="14" hidden="1" x14ac:dyDescent="0.15">
       <c r="A58" s="5" t="s">
         <v>68</v>
       </c>
@@ -4276,7 +4347,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="42" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:8" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.15">
       <c r="A59" s="5" t="s">
         <v>68</v>
       </c>
@@ -4299,30 +4370,31 @@
         <v>234</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="14" x14ac:dyDescent="0.15">
-      <c r="A60" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B60" s="5" t="s">
+    <row r="60" spans="1:8" s="18" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A60" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B60" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="C60" s="5">
-        <v>1</v>
-      </c>
-      <c r="D60" s="5">
-        <v>8</v>
-      </c>
-      <c r="E60" s="5" t="s">
+      <c r="C60" s="21">
+        <v>1</v>
+      </c>
+      <c r="D60" s="21">
+        <v>8</v>
+      </c>
+      <c r="E60" s="21" t="s">
         <v>190</v>
       </c>
-      <c r="F60" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="G60" s="6" t="s">
+      <c r="F60" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="G60" s="22" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" ht="14" x14ac:dyDescent="0.15">
+      <c r="H60" s="15"/>
+    </row>
+    <row r="61" spans="1:8" customFormat="1" ht="14" hidden="1" x14ac:dyDescent="0.15">
       <c r="A61" s="5" t="s">
         <v>68</v>
       </c>
@@ -4345,7 +4417,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="62" spans="1:8" s="16" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:8" s="12" customFormat="1" ht="14" hidden="1" x14ac:dyDescent="0.15">
       <c r="A62" s="5" t="s">
         <v>68</v>
       </c>
@@ -4368,7 +4440,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="63" spans="1:8" s="16" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:8" s="12" customFormat="1" ht="14" hidden="1" x14ac:dyDescent="0.15">
       <c r="A63" s="5" t="s">
         <v>68</v>
       </c>
@@ -4389,7 +4461,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="56" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:8" customFormat="1" ht="56" hidden="1" x14ac:dyDescent="0.15">
       <c r="A64" s="5" t="s">
         <v>68</v>
       </c>
@@ -4409,7 +4481,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="70" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:8" customFormat="1" ht="70" hidden="1" x14ac:dyDescent="0.15">
       <c r="A65" s="5" t="s">
         <v>68</v>
       </c>
@@ -4432,7 +4504,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="409.6" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:8" customFormat="1" ht="409.6" hidden="1" x14ac:dyDescent="0.15">
       <c r="A66" s="5" t="s">
         <v>68</v>
       </c>
@@ -4452,7 +4524,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="98" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:8" customFormat="1" ht="98" hidden="1" x14ac:dyDescent="0.15">
       <c r="A67" s="5" t="s">
         <v>68</v>
       </c>
@@ -4472,7 +4544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="56" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:8" customFormat="1" ht="56" hidden="1" x14ac:dyDescent="0.15">
       <c r="A68" s="5" t="s">
         <v>68</v>
       </c>
@@ -4495,30 +4567,31 @@
         <v>108</v>
       </c>
     </row>
-    <row r="69" spans="1:8" s="16" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="A69" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B69" s="5" t="s">
+    <row r="69" spans="1:8" s="18" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A69" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B69" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="C69" s="5">
-        <v>1</v>
-      </c>
-      <c r="D69" s="5">
-        <v>8</v>
-      </c>
-      <c r="E69" s="5" t="s">
+      <c r="C69" s="21">
+        <v>1</v>
+      </c>
+      <c r="D69" s="21">
+        <v>8</v>
+      </c>
+      <c r="E69" s="21" t="s">
         <v>287</v>
       </c>
-      <c r="F69" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="G69" s="6" t="s">
+      <c r="F69" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="G69" s="22" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" ht="14" x14ac:dyDescent="0.15">
+      <c r="H69" s="15"/>
+    </row>
+    <row r="70" spans="1:8" customFormat="1" ht="14" hidden="1" x14ac:dyDescent="0.15">
       <c r="A70" s="5" t="s">
         <v>68</v>
       </c>
@@ -4541,7 +4614,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="71" spans="1:8" s="16" customFormat="1" ht="56" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:8" s="12" customFormat="1" ht="56" hidden="1" x14ac:dyDescent="0.15">
       <c r="A71" s="5" t="s">
         <v>68</v>
       </c>
@@ -4562,7 +4635,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:8" customFormat="1" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A72" s="5" t="s">
         <v>68</v>
       </c>
@@ -4585,7 +4658,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="73" spans="1:8" s="16" customFormat="1" ht="70" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:8" s="12" customFormat="1" ht="70" hidden="1" x14ac:dyDescent="0.15">
       <c r="A73" s="5" t="s">
         <v>68</v>
       </c>
@@ -4608,7 +4681,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="56" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:8" s="15" customFormat="1" ht="56" hidden="1" x14ac:dyDescent="0.15">
       <c r="A74" s="5" t="s">
         <v>68</v>
       </c>
@@ -4627,8 +4700,9 @@
       <c r="G74" s="6" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" ht="14" x14ac:dyDescent="0.15">
+      <c r="H74" s="14"/>
+    </row>
+    <row r="75" spans="1:8" customFormat="1" ht="14" hidden="1" x14ac:dyDescent="0.15">
       <c r="A75" s="5" t="s">
         <v>68</v>
       </c>
@@ -4652,29 +4726,29 @@
       </c>
       <c r="H75" s="7"/>
     </row>
-    <row r="76" spans="1:8" s="16" customFormat="1" ht="70" x14ac:dyDescent="0.15">
-      <c r="A76" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B76" s="5" t="s">
+    <row r="76" spans="1:8" s="18" customFormat="1" ht="70" x14ac:dyDescent="0.15">
+      <c r="A76" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B76" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="C76" s="5">
-        <v>1</v>
-      </c>
-      <c r="D76" s="5">
-        <v>8</v>
-      </c>
-      <c r="E76" s="5" t="s">
+      <c r="C76" s="21">
+        <v>1</v>
+      </c>
+      <c r="D76" s="21">
+        <v>8</v>
+      </c>
+      <c r="E76" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="F76"/>
-      <c r="G76" s="6" t="s">
+      <c r="F76" s="23"/>
+      <c r="G76" s="22" t="s">
         <v>173</v>
       </c>
-      <c r="H76" s="18"/>
-    </row>
-    <row r="77" spans="1:8" ht="42" x14ac:dyDescent="0.15">
+      <c r="H76" s="7"/>
+    </row>
+    <row r="77" spans="1:8" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.15">
       <c r="A77" s="5" t="s">
         <v>68</v>
       </c>
@@ -4694,7 +4768,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="14" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:8" customFormat="1" ht="14" hidden="1" x14ac:dyDescent="0.15">
       <c r="A78" s="5" t="s">
         <v>68</v>
       </c>
@@ -4714,7 +4788,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="56" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:8" customFormat="1" ht="56" hidden="1" x14ac:dyDescent="0.15">
       <c r="A79" s="5" t="s">
         <v>68</v>
       </c>
@@ -4738,10 +4812,10 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A79">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G79">
-      <sortCondition sortBy="cellColor" ref="A1:A79" dxfId="1"/>
-    </sortState>
+  <autoFilter ref="A1:G79" xr:uid="{00000000-0001-0000-0200-000000000000}">
+    <filterColumn colId="1">
+      <colorFilter dxfId="0"/>
+    </filterColumn>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -4750,7 +4824,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -5236,7 +5310,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -5832,7 +5906,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H77"/>
   <sheetViews>
     <sheetView topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">

</xml_diff>